<commit_message>
change approved_date to uploaded_date
</commit_message>
<xml_diff>
--- a/Contractor-Plans.xlsx
+++ b/Contractor-Plans.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P4"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,75 +436,80 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t xml:space="preserve">Mã KHLCNT </t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>Tên Chủ đầu tư</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Tên gói thầu</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Tóm tắt công việc chính</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Lĩnh vực</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Giá gói thầu (VND)</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Chi tiết nguồn vốn</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Hình thức LCNT</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Phương thức LCNT</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Thời gian tổ chức LCNT</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Thời gian bắt đầu tổ chức LCNT</t>
         </is>
       </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>Loại hợp đồng</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="N1" s="1" t="inlineStr">
         <is>
           <t>Thời gian thức hiện gói thầu</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="O1" s="1" t="inlineStr">
         <is>
           <t>Tùy chọn mua thêm</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="P1" s="1" t="inlineStr">
         <is>
           <t>Giám sát hoạt động đấu thầu (nếu có)</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
+      <c r="Q1" s="1" t="inlineStr">
         <is>
           <t>Tình trạng TBMT</t>
         </is>
@@ -516,75 +521,80 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>PL2400235573-00</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
           <t>CÔNG TY CỔ PHẦN THỦY ĐIỆN THÁC MƠ</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2024-TMPIT-06.08. Mua phần mềm ZWCAD 2D phiên bản Std</t>
-        </is>
-      </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>Mua phần mềm ZWCAD 2D phiên bản Std</t>
+          <t>2024-TMPCT-19.39: Sửa chữa lớn Đường vận hành Nhà máy điện mặt trời Thác Mơ - Khu 1.1, 1.2 và Khu 6</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Hàng hóa</t>
+          <t>Sửa chữa mặt đường tại khu vực 1.1, 1.2 và Khu 6</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>87.600.000</t>
+          <t>Xây lắp</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Vốn SXKD năm 2024</t>
+          <t>6.618.037.829</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Chào hàng cạnh tranh</t>
+          <t>SXKD 2025</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
+          <t>Đấu thầu rộng rãi</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
           <t>Một giai đoạn một túi hồ sơ</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>50 ngày</t>
-        </is>
-      </c>
       <c r="K2" t="inlineStr">
         <is>
+          <t>60 ngày</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
           <t>Quý IV, 2024</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>Trọn gói</t>
         </is>
       </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t>30 ngày</t>
-        </is>
-      </c>
       <c r="N2" t="inlineStr">
         <is>
+          <t>90 ngày</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
           <t>Không</t>
         </is>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Không có</t>
-        </is>
-      </c>
       <c r="P2" t="inlineStr">
+        <is>
+          <t>Không</t>
+        </is>
+      </c>
+      <c r="Q2" t="inlineStr">
         <is>
           <t>Chưa có TBMT</t>
         </is>
@@ -596,71 +606,80 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>PL2400223718-00</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>CÔNG TY CỔ PHẦN THỦY ĐIỆN THÁC MƠ</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2024-TMP-TB-10.28. Cung cấp và lắp đặt hệ thống giám sát trực tuyến rung đảo cho tổ máy số 2 Nhà máy Thủy điện Thác Mơ</t>
-        </is>
-      </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Cung cấp, lắp đặt hệ thống giám sát trực tuyến rung đảo cho tổ máy H2 Nhà máy Thủy điện Thác Mơ</t>
+          <t>2024-TMPIT-06.08. Mua phần mềm ZWCAD 2D phiên bản Std</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
+          <t>Mua phần mềm ZWCAD 2D phiên bản Std</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>Hàng hóa</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>4.945.499.274</t>
-        </is>
-      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Đầu tư phát triển</t>
+          <t>87.600.000</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Đấu thầu rộng rãi</t>
+          <t>Vốn SXKD năm 2024</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
         <is>
+          <t>Chào hàng cạnh tranh</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
           <t>Một giai đoạn một túi hồ sơ</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>65 ngày</t>
-        </is>
-      </c>
       <c r="K3" t="inlineStr">
         <is>
+          <t>50 ngày</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
           <t>Quý IV, 2024</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr">
+      <c r="M3" t="inlineStr">
         <is>
           <t>Trọn gói</t>
         </is>
       </c>
-      <c r="M3" t="inlineStr">
-        <is>
-          <t>120 ngày</t>
-        </is>
-      </c>
       <c r="N3" t="inlineStr">
         <is>
+          <t>30 ngày</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
           <t>Không</t>
         </is>
       </c>
-      <c r="O3" t="inlineStr"/>
       <c r="P3" t="inlineStr">
+        <is>
+          <t>Không có</t>
+        </is>
+      </c>
+      <c r="Q3" t="inlineStr">
         <is>
           <t>Chưa có TBMT</t>
         </is>
@@ -672,71 +691,157 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>PL2400222451-00</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
           <t>CÔNG TY CỔ PHẦN THỦY ĐIỆN THÁC MƠ</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2024-TMP-TB-10.28. Cung cấp và lắp đặt hệ thống giám sát trực tuyến rung đảo cho tổ máy số 2 Nhà máy Thủy điện Thác Mơ</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Cung cấp, lắp đặt hệ thống giám sát trực tuyến rung đảo cho tổ máy H2 Nhà máy Thủy điện Thác Mơ</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Hàng hóa</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>4.945.499.274</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Đầu tư phát triển</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Đấu thầu rộng rãi</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Một giai đoạn một túi hồ sơ</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>65 ngày</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>Quý IV, 2024</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>Trọn gói</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>120 ngày</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>Không</t>
+        </is>
+      </c>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>Chưa có TBMT</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>PL2400222451-00</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>CÔNG TY CỔ PHẦN THỦY ĐIỆN THÁC MƠ</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>2024-TMP-TB-10.29. Cung cấp và lắp đặt hệ thống giám sát phóng điện cục bộ (PD) cho tổ máy số 2 Nhà máy Thủy điện Thác Mơ</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>Cung cấp, lắp đặt hệ thống giám sát phóng điện cục bộ cho tổ máy H2 Nhà máy Thủy điện Thác Mơ</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>Hàng hóa</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>4.881.690.001</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>Đầu tư phát triển</t>
         </is>
       </c>
-      <c r="H4" t="inlineStr">
+      <c r="I5" t="inlineStr">
         <is>
           <t>Đấu thầu rộng rãi</t>
         </is>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>Một giai đoạn một túi hồ sơ</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
+      <c r="K5" t="inlineStr">
         <is>
           <t>65 ngày</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>Quý IV, 2024</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>Trọn gói</t>
         </is>
       </c>
-      <c r="M4" t="inlineStr">
+      <c r="N5" t="inlineStr">
         <is>
           <t>140 ngày</t>
         </is>
       </c>
-      <c r="N4" t="inlineStr">
+      <c r="O5" t="inlineStr">
         <is>
           <t>Không</t>
         </is>
       </c>
-      <c r="O4" t="inlineStr"/>
-      <c r="P4" t="inlineStr">
+      <c r="P5" t="inlineStr"/>
+      <c r="Q5" t="inlineStr">
         <is>
           <t>Chưa có TBMT</t>
         </is>

</xml_diff>